<commit_message>
Basic Mouseover for Inventory
</commit_message>
<xml_diff>
--- a/Documents/Guppen-Planung.xlsx
+++ b/Documents/Guppen-Planung.xlsx
@@ -365,9 +365,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -405,7 +405,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +477,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -654,7 +654,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,21 +1191,21 @@
         <v>6</v>
       </c>
       <c r="C18" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D18" s="4">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="H18" s="12" t="str">
         <f t="shared" si="3"/>
@@ -1221,10 +1221,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Documents Updated + 1 Level expanded (Mountian Finished)
</commit_message>
<xml_diff>
--- a/Documents/Guppen-Planung.xlsx
+++ b/Documents/Guppen-Planung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Sascha, Cedric</t>
+  </si>
+  <si>
+    <t>Implementation of First Boss ("Witch Tree") with Squirel</t>
+  </si>
+  <si>
+    <t>Combatsystem for Axe</t>
   </si>
 </sst>
 </file>
@@ -654,7 +660,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,22 +1078,22 @@
         <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="1"/>
-        <v>0.66666666666666674</v>
+        <v>1</v>
       </c>
       <c r="H14" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I14" s="5"/>
     </row>
@@ -1244,27 +1250,37 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="4">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <v>10</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>X</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B21" s="4"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>

</xml_diff>